<commit_message>
update code newest for check tool heyK
</commit_message>
<xml_diff>
--- a/src/excel/Check Error HeyKorea_Dữ liệu trung cấp.xlsx
+++ b/src/excel/Check Error HeyKorea_Dữ liệu trung cấp.xlsx
@@ -7,7 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="100_Du lịch (2)" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="143_Cư trú" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="142_Phân loại rác" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="141_Sinh hoạt hàng ngày" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -423,4 +425,40 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>